<commit_message>
add balance and label sheet
</commit_message>
<xml_diff>
--- a/AccountBooks/KeepAccountDataBase.xlsx
+++ b/AccountBooks/KeepAccountDataBase.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PythonFiles\KeepAccounts\KeepAccounts_20230204\KeepAccounts_v2.0\AccountBooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3B892D-38E4-4D96-8597-45C0E7BD5463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2441241-C3A5-419E-9A46-7903C588A873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3735" windowWidth="28215" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Records" sheetId="2" r:id="rId1"/>
+    <sheet name="余额" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Records!$A$1:$J$1</definedName>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>来源</t>
   </si>
@@ -87,17 +88,61 @@
     <t>修订金额</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>微信</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>财付通</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支付宝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>银行卡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工资卡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>现金</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>公积金</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>余额宝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="yyyy/m/d\ h:mm;@"/>
     <numFmt numFmtId="178" formatCode="0.00_ ;[Red]\-0.00\ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,8 +167,22 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +192,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF647FBC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -171,7 +236,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -196,6 +261,18 @@
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -975,10 +1052,10 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.125" style="8" customWidth="1"/>
     <col min="2" max="2" width="7.75" style="2" bestFit="1" customWidth="1"/>
@@ -992,7 +1069,7 @@
     <col min="10" max="10" width="23.5" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
@@ -1025,43 +1102,915 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J1">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:J1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A2:G47041 I2:J47041">
-    <cfRule type="expression" dxfId="5" priority="43">
+    <cfRule type="expression" dxfId="5" priority="46">
       <formula>AND(#REF!=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="44">
+    <cfRule type="expression" dxfId="4" priority="47">
       <formula>AND(#REF!&lt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="45">
+    <cfRule type="expression" dxfId="3" priority="48">
       <formula>AND(#REF!&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H47041">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>AND(#REF!=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>AND(#REF!&lt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>AND(#REF!&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
-      <formula1>INDIRECT($I$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
-      <formula1>INDIRECT(I2)</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BEB8663-6132-4ED8-81A5-837493C602C4}">
+  <dimension ref="A1:K38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="11" max="11" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
+        <v>43845</v>
+      </c>
+      <c r="K2">
+        <v>4255.62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
+        <v>43876</v>
+      </c>
+      <c r="K3">
+        <v>4024.92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
+        <v>43905</v>
+      </c>
+      <c r="K4">
+        <v>5131.17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>43936</v>
+      </c>
+      <c r="K5">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
+        <v>43966</v>
+      </c>
+      <c r="K6">
+        <v>5882</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>43997</v>
+      </c>
+      <c r="K7">
+        <v>4476.4799999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
+        <v>44027</v>
+      </c>
+      <c r="K8">
+        <v>5240.49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>44058</v>
+      </c>
+      <c r="K9">
+        <v>5939.88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>44089</v>
+      </c>
+      <c r="K10">
+        <v>6232.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>44119</v>
+      </c>
+      <c r="K11">
+        <v>5446.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>44150</v>
+      </c>
+      <c r="K12">
+        <v>4208.38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>44180</v>
+      </c>
+      <c r="K13">
+        <v>6492</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="9">
+        <v>44211</v>
+      </c>
+      <c r="K14">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>44256</v>
+      </c>
+      <c r="B15">
+        <v>30.32</v>
+      </c>
+      <c r="C15">
+        <v>1173.05</v>
+      </c>
+      <c r="D15">
+        <v>1350</v>
+      </c>
+      <c r="E15">
+        <v>1848.52</v>
+      </c>
+      <c r="F15">
+        <v>682.22</v>
+      </c>
+      <c r="H15">
+        <v>1300</v>
+      </c>
+      <c r="J15">
+        <v>43.44</v>
+      </c>
+      <c r="K15">
+        <f t="shared" ref="K15:K37" si="0">SUM(B15:J15)</f>
+        <v>6427.5499999999993</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>44287</v>
+      </c>
+      <c r="B16">
+        <v>0.22</v>
+      </c>
+      <c r="C16">
+        <v>9973.49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16">
+        <v>1335.1</v>
+      </c>
+      <c r="F16">
+        <v>6.4</v>
+      </c>
+      <c r="H16">
+        <v>1612</v>
+      </c>
+      <c r="J16">
+        <v>82.86</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>13010.07</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>44317</v>
+      </c>
+      <c r="B17">
+        <v>0.62</v>
+      </c>
+      <c r="C17">
+        <v>8105.95</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>1386.55</v>
+      </c>
+      <c r="F17">
+        <v>1431.31</v>
+      </c>
+      <c r="H17">
+        <v>112</v>
+      </c>
+      <c r="J17">
+        <v>44.9</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>11081.329999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>44348</v>
+      </c>
+      <c r="B18">
+        <v>9.66</v>
+      </c>
+      <c r="C18">
+        <v>8411</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <v>2300.13</v>
+      </c>
+      <c r="F18">
+        <v>88.56</v>
+      </c>
+      <c r="H18">
+        <v>102</v>
+      </c>
+      <c r="J18">
+        <v>37.770000000000003</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>10949.12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="9">
+        <v>44378</v>
+      </c>
+      <c r="B19">
+        <v>1.65</v>
+      </c>
+      <c r="C19">
+        <v>7612.64</v>
+      </c>
+      <c r="D19">
+        <v>16.93</v>
+      </c>
+      <c r="E19">
+        <v>2397.54</v>
+      </c>
+      <c r="F19">
+        <v>853.6</v>
+      </c>
+      <c r="H19">
+        <v>102</v>
+      </c>
+      <c r="J19">
+        <v>35.82</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>11020.18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="9">
+        <v>44409</v>
+      </c>
+      <c r="B20">
+        <v>3.77</v>
+      </c>
+      <c r="C20">
+        <v>5585.72</v>
+      </c>
+      <c r="D20">
+        <v>20.07</v>
+      </c>
+      <c r="E20">
+        <v>3457.71</v>
+      </c>
+      <c r="F20">
+        <v>18.3</v>
+      </c>
+      <c r="H20">
+        <v>102</v>
+      </c>
+      <c r="J20">
+        <v>12.5</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>9200.07</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="9">
+        <v>44440</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>2466.7600000000002</v>
+      </c>
+      <c r="D21">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="E21">
+        <v>3462.85</v>
+      </c>
+      <c r="F21">
+        <v>30.78</v>
+      </c>
+      <c r="H21">
+        <v>101</v>
+      </c>
+      <c r="J21">
+        <v>90.14</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>6156.55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="9">
+        <v>44470</v>
+      </c>
+      <c r="B22">
+        <v>1.6</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>2993.65</v>
+      </c>
+      <c r="F22">
+        <v>808.96</v>
+      </c>
+      <c r="H22">
+        <v>101</v>
+      </c>
+      <c r="J22">
+        <v>13</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>3918.21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="9">
+        <v>44501</v>
+      </c>
+      <c r="B23">
+        <v>0.49</v>
+      </c>
+      <c r="C23">
+        <v>2124.31</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>2830.89</v>
+      </c>
+      <c r="F23">
+        <v>568.26</v>
+      </c>
+      <c r="H23">
+        <v>111</v>
+      </c>
+      <c r="J23">
+        <v>1.94</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>5636.8899999999994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="9">
+        <v>44531</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>3585.58</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>2851.2</v>
+      </c>
+      <c r="F24">
+        <v>6.68</v>
+      </c>
+      <c r="H24">
+        <v>111</v>
+      </c>
+      <c r="J24">
+        <v>91.51</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>6645.97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="9">
+        <v>44562</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>11053.869999999999</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>3170.21</v>
+      </c>
+      <c r="F25">
+        <v>7.71</v>
+      </c>
+      <c r="H25">
+        <v>111</v>
+      </c>
+      <c r="J25">
+        <v>84.66</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>14427.449999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="9">
+        <v>44593</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>9028.43</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>4040.71</v>
+      </c>
+      <c r="F26">
+        <v>62.56</v>
+      </c>
+      <c r="H26">
+        <v>111</v>
+      </c>
+      <c r="J26">
+        <v>77.87</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>13320.57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="9">
+        <v>44621</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>7905.52</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>4845.78</v>
+      </c>
+      <c r="F27">
+        <v>51.57</v>
+      </c>
+      <c r="H27">
+        <v>111</v>
+      </c>
+      <c r="J27">
+        <v>45.92</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>12959.789999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="9">
+        <v>44652</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>7866.24</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>3516.56</v>
+      </c>
+      <c r="F28">
+        <v>169.12</v>
+      </c>
+      <c r="H28">
+        <v>111</v>
+      </c>
+      <c r="J28">
+        <v>25.14</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>11688.06</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="9">
+        <v>44682</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>6029.21</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>3529.51</v>
+      </c>
+      <c r="F29">
+        <v>27.69</v>
+      </c>
+      <c r="H29">
+        <v>111</v>
+      </c>
+      <c r="J29">
+        <v>4.2</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>9701.6100000000024</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="9">
+        <v>44713</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>20048.05</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>3401.66</v>
+      </c>
+      <c r="F30">
+        <v>9.66</v>
+      </c>
+      <c r="H30">
+        <v>111</v>
+      </c>
+      <c r="J30">
+        <v>62.24</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>23632.61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="9">
+        <v>44721</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>17074.41</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>3421.97</v>
+      </c>
+      <c r="F31">
+        <v>1043.03</v>
+      </c>
+      <c r="H31">
+        <v>111</v>
+      </c>
+      <c r="J31">
+        <v>22.38</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>21672.79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="9">
+        <v>44750</v>
+      </c>
+      <c r="B32">
+        <v>2.35</v>
+      </c>
+      <c r="C32">
+        <v>5674.05</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>3364.97</v>
+      </c>
+      <c r="F32">
+        <v>152.22999999999999</v>
+      </c>
+      <c r="H32">
+        <v>1188</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>10381.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="9">
+        <v>44776</v>
+      </c>
+      <c r="B33">
+        <v>2.93</v>
+      </c>
+      <c r="C33">
+        <v>1218.04</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>2858.31</v>
+      </c>
+      <c r="F33">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G33">
+        <v>19782.04</v>
+      </c>
+      <c r="H33">
+        <v>1188</v>
+      </c>
+      <c r="I33">
+        <v>2000</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="0"/>
+        <v>27050.420000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="9">
+        <v>44822</v>
+      </c>
+      <c r="B34">
+        <v>0.31</v>
+      </c>
+      <c r="C34">
+        <v>9.4600000000000009</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>22331.15</v>
+      </c>
+      <c r="F34">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G34">
+        <v>21006.62</v>
+      </c>
+      <c r="H34">
+        <v>1188</v>
+      </c>
+      <c r="I34">
+        <v>4000</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="0"/>
+        <v>48536.639999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="9">
+        <v>44835</v>
+      </c>
+      <c r="B35">
+        <v>4.25</v>
+      </c>
+      <c r="C35">
+        <v>0.76</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>41330.28</v>
+      </c>
+      <c r="F35">
+        <v>0.12</v>
+      </c>
+      <c r="G35">
+        <v>19430.230000000003</v>
+      </c>
+      <c r="H35">
+        <v>1188</v>
+      </c>
+      <c r="I35">
+        <v>6000</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>67953.640000000014</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="9">
+        <v>44888</v>
+      </c>
+      <c r="B36">
+        <v>143.09</v>
+      </c>
+      <c r="C36">
+        <v>0.76</v>
+      </c>
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36">
+        <v>72549.62</v>
+      </c>
+      <c r="F36">
+        <v>0.12</v>
+      </c>
+      <c r="G36">
+        <v>768</v>
+      </c>
+      <c r="H36">
+        <v>1188</v>
+      </c>
+      <c r="I36">
+        <v>8000</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="0"/>
+        <v>82649.59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="9">
+        <v>44910</v>
+      </c>
+      <c r="B37">
+        <v>6.22</v>
+      </c>
+      <c r="C37">
+        <v>0.76</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37">
+        <v>60260.99</v>
+      </c>
+      <c r="F37">
+        <v>0.12</v>
+      </c>
+      <c r="G37">
+        <v>20201.240000000002</v>
+      </c>
+      <c r="H37">
+        <v>1188</v>
+      </c>
+      <c r="I37">
+        <v>12000</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="0"/>
+        <v>93657.33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="9">
+        <v>44927</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>